<commit_message>
Finish intro and data
</commit_message>
<xml_diff>
--- a/04 - Project/Project 1 Checklist.xlsx
+++ b/04 - Project/Project 1 Checklist.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive\Documents\Github\Intro_to_R_DSA-5011\04 - Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B2A12F-B21A-4D16-BE29-81161B848C5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F959CE-BDB9-440D-BBB0-A4F9F7788CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F11A0DD-2F4C-4095-89C7-8CE9C716C55F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6F11A0DD-2F4C-4095-89C7-8CE9C716C55F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" calcOnSave="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">1) Plot the data with the fitted line – you can use any package you want – ggplot would work well. 2) The plot can be made to appear when the function is used. 3) The plot should be saved to the working directory as well (automatic). use ggsave(), png(), jpeg() etc
 </t>
@@ -73,6 +74,81 @@
   </si>
   <si>
     <t>Written?</t>
+  </si>
+  <si>
+    <t>mpg</t>
+  </si>
+  <si>
+    <t>Miles/(US) gallon</t>
+  </si>
+  <si>
+    <t>cyl</t>
+  </si>
+  <si>
+    <t>Number of cylinders</t>
+  </si>
+  <si>
+    <t>disp</t>
+  </si>
+  <si>
+    <t>Displacement (cu.in.)</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>Gross horsepower</t>
+  </si>
+  <si>
+    <t>drat</t>
+  </si>
+  <si>
+    <t>Rear axle ratio</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>Weight (1000 lbs)</t>
+  </si>
+  <si>
+    <t>qsec</t>
+  </si>
+  <si>
+    <t>1/4 mile time</t>
+  </si>
+  <si>
+    <t>vs</t>
+  </si>
+  <si>
+    <t>Engine (0 = V-shaped, 1 = straight)</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>Transmission (0 = automatic, 1 = manual)</t>
+  </si>
+  <si>
+    <t>gear</t>
+  </si>
+  <si>
+    <t>Number of forward gears</t>
+  </si>
+  <si>
+    <t>carb</t>
+  </si>
+  <si>
+    <t>Number of carburetors</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Variable Description</t>
+  </si>
+  <si>
+    <t>Data Type</t>
   </si>
 </sst>
 </file>
@@ -503,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF187EA0-956D-435D-852C-0C1924C1CDB1}">
   <dimension ref="A3:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,4 +735,122 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5057CA-4BBF-484E-A0B5-4F17ECBA7DE2}">
+  <dimension ref="B2:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Polished LM Function and rmd
</commit_message>
<xml_diff>
--- a/04 - Project/Project 1 Checklist.xlsx
+++ b/04 - Project/Project 1 Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive\Documents\Github\Intro_to_R_DSA-5011\04 - Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F959CE-BDB9-440D-BBB0-A4F9F7788CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3371C37-5876-4650-AA26-B4D0C370F393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6F11A0DD-2F4C-4095-89C7-8CE9C716C55F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F11A0DD-2F4C-4095-89C7-8CE9C716C55F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t xml:space="preserve">1) Plot the data with the fitted line – you can use any package you want – ggplot would work well. 2) The plot can be made to appear when the function is used. 3) The plot should be saved to the working directory as well (automatic). use ggsave(), png(), jpeg() etc
 </t>
@@ -149,6 +149,51 @@
   </si>
   <si>
     <t>Data Type</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>Nominal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Represents the dependant, or explained, variable.</t>
+  </si>
+  <si>
+    <t>\begin{equation}\beta_{0}\end{equation}</t>
+  </si>
+  <si>
+    <t>represents the estimated intercept.</t>
+  </si>
+  <si>
+    <t>\begin{equation}\beta_{i}\end{equation}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> represents the slope of the estimated vector.</t>
+  </si>
+  <si>
+    <t>\begin{equation}X_{i}\end{equation}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> represents the independent, or control, variable.</t>
+  </si>
+  <si>
+    <t>\begin{equation}\epsilon_{i}\end{equation}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> represents some error term.</t>
+  </si>
+  <si>
+    <t>\begin{equation}Y\end{equation}</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -579,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF187EA0-956D-435D-852C-0C1924C1CDB1}">
   <dimension ref="A3:J12"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,14 +674,16 @@
       <c r="C5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E5" t="b">
         <f t="shared" ref="E5:E12" si="0">IFERROR(AND(
 IF(C5 = "", FALSE, C5),
 IF(D5 = "", FALSE, D5)
 ),
 FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -646,10 +693,12 @@
       <c r="C6" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E6" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -659,10 +708,12 @@
       <c r="C7" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E7" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -672,10 +723,12 @@
       <c r="C8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E8" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="60" x14ac:dyDescent="0.25">
@@ -685,9 +738,12 @@
       <c r="C9" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="D9" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="E9" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -724,12 +780,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>F1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>E1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -739,10 +795,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5057CA-4BBF-484E-A0B5-4F17ECBA7DE2}">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,6 +824,9 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -776,6 +835,9 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -784,6 +846,9 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -792,6 +857,9 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -800,6 +868,9 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -808,6 +879,9 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -816,6 +890,9 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -824,6 +901,9 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -832,6 +912,9 @@
       <c r="C11" t="s">
         <v>29</v>
       </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -840,6 +923,9 @@
       <c r="C12" t="s">
         <v>31</v>
       </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -847,6 +933,57 @@
       </c>
       <c r="C13" t="s">
         <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>